<commit_message>
mise à jour des notebook transport
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_acier_1D_2050.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_acier_1D_2050.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F07161A-BC4C-CA43-8BA6-BD9493B5E9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0522DD65-3ADF-5841-B84A-228C299033C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="4180" windowWidth="34040" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9920" yWindow="500" windowWidth="28800" windowHeight="13720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="2" r:id="rId1"/>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
@@ -929,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2933DD02-9F7C-6142-84AA-FCB2689DBD13}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1093,7 +1093,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>